<commit_message>
updating some results during rivanna maintenence
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Documents\UVA\research\rl_surveillance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackheavey/Documents/UVA/research/rl_surveillance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13C3BD7-0809-47FA-B887-3BC2D8D26C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96267151-EC64-3A44-987E-6DF06EC2448E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{258ED805-0B0A-492C-A0D4-21D8563E75EA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{258ED805-0B0A-492C-A0D4-21D8563E75EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="initial results" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -107,7 +103,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,13 +111,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,13 +165,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,467 +493,643 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65A1FC8-AF5A-42E8-A135-5B32DA0EB66B}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>0.01</v>
-      </c>
-      <c r="C2">
-        <v>0.01</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="2">
         <v>47175894</v>
       </c>
-      <c r="K2" t="s">
+      <c r="F2" s="2">
+        <v>-9724.07</v>
+      </c>
+      <c r="G2" s="2">
+        <v>770.71</v>
+      </c>
+      <c r="L2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>0.01</v>
-      </c>
-      <c r="C3">
-        <v>0.01</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="2">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E3" s="2">
         <v>47175895</v>
       </c>
-      <c r="K3" t="s">
+      <c r="F3" s="2">
+        <v>-9936.64</v>
+      </c>
+      <c r="G3" s="2">
+        <v>814.09067000000005</v>
+      </c>
+      <c r="L3" t="s">
         <v>5</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>202</v>
       </c>
-      <c r="M3">
-        <f>L3*101</f>
+      <c r="N3">
+        <f>M3*101</f>
         <v>20402</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4">
-        <v>0.01</v>
-      </c>
-      <c r="C4">
-        <v>0.01</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="2">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E4" s="2">
         <v>47175895</v>
       </c>
-      <c r="K4" t="s">
+      <c r="F4" s="2">
+        <v>-9831.48</v>
+      </c>
+      <c r="G4" s="2">
+        <v>648.69500000000005</v>
+      </c>
+      <c r="L4" t="s">
         <v>6</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>692</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5">
-        <v>0.01</v>
-      </c>
-      <c r="C5">
-        <v>0.01</v>
-      </c>
-      <c r="D5">
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="2">
         <v>47175895</v>
       </c>
-      <c r="K5" t="s">
+      <c r="F5" s="2">
+        <v>-9723.92</v>
+      </c>
+      <c r="G5" s="2">
+        <v>713.31176000000005</v>
+      </c>
+      <c r="L5" t="s">
         <v>8</v>
       </c>
-      <c r="L5">
+      <c r="M5" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E6" s="3">
+        <v>47174758</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-13718.5766</v>
+      </c>
+      <c r="G6" s="3">
+        <v>368.00659999999999</v>
+      </c>
+      <c r="L6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" s="3">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E7" s="3">
+        <v>47174759</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="L7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E8" s="3">
+        <v>47174759</v>
+      </c>
+      <c r="F8" s="3">
+        <v>-13942.5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>380.81200000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E9" s="3">
+        <v>47174759</v>
+      </c>
+      <c r="F9" s="3">
+        <v>-13888.7</v>
+      </c>
+      <c r="G9" s="3">
+        <v>343.31099999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0.03</v>
-      </c>
-      <c r="C6">
-        <v>0.03</v>
-      </c>
-      <c r="D6">
-        <v>47174758</v>
-      </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B10" s="1">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E10" s="1">
+        <v>47174791</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-15884.336600000001</v>
+      </c>
+      <c r="G10" s="1">
+        <v>210.6748</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7">
-        <v>0.03</v>
-      </c>
-      <c r="C7">
-        <v>0.03</v>
-      </c>
-      <c r="D7">
-        <v>47174759</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B11" s="1">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E11" s="1">
+        <v>47174797</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8">
-        <v>0.03</v>
-      </c>
-      <c r="C8">
-        <v>0.03</v>
-      </c>
-      <c r="D8">
-        <v>47174759</v>
-      </c>
-      <c r="E8">
-        <v>-13942.5</v>
-      </c>
-      <c r="F8">
-        <v>380.81200000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>0.03</v>
-      </c>
-      <c r="C9">
-        <v>0.03</v>
-      </c>
-      <c r="D9">
-        <v>47174759</v>
-      </c>
-      <c r="E9">
-        <v>-13888.7</v>
-      </c>
-      <c r="F9">
-        <v>343.31099999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B12" s="1">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E12" s="1">
+        <v>47174797</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-16068.08</v>
+      </c>
+      <c r="G12" s="1">
+        <v>231.601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E13" s="1">
+        <v>47174797</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-16081.8</v>
+      </c>
+      <c r="G13" s="1">
+        <v>237.786</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
-        <v>0.05</v>
-      </c>
-      <c r="C10">
-        <v>0.03</v>
-      </c>
-      <c r="D10">
-        <v>47174791</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B14" s="2">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E14" s="2">
+        <v>47175166</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-16906.973300000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>175.23859999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
-        <v>0.05</v>
-      </c>
-      <c r="C11">
-        <v>0.03</v>
-      </c>
-      <c r="D11">
-        <v>47174797</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B15" s="2">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E15" s="2">
+        <v>47175169</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12">
-        <v>0.05</v>
-      </c>
-      <c r="C12">
-        <v>0.03</v>
-      </c>
-      <c r="D12">
-        <v>47174797</v>
-      </c>
-      <c r="E12">
-        <v>-16068.08</v>
-      </c>
-      <c r="F12">
-        <v>231.601</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>0.05</v>
-      </c>
-      <c r="C13">
-        <v>0.03</v>
-      </c>
-      <c r="D13">
-        <v>47174797</v>
-      </c>
-      <c r="E13">
-        <v>-16081.8</v>
-      </c>
-      <c r="F13">
-        <v>237.786</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B16" s="2">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E16" s="2">
+        <v>47175169</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-17102.3</v>
+      </c>
+      <c r="G16" s="2">
+        <v>182.774</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E17" s="2">
+        <v>47175169</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-17058.259999999998</v>
+      </c>
+      <c r="G17" s="2">
+        <v>149.58099999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B14">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C14">
-        <v>0.03</v>
-      </c>
-      <c r="D14">
-        <v>47175166</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B18" s="3">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E18" s="3">
+        <v>47175426</v>
+      </c>
+      <c r="F18" s="3">
+        <v>-17495.796600000001</v>
+      </c>
+      <c r="G18" s="3">
+        <v>132.8047</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C15">
-        <v>0.03</v>
-      </c>
-      <c r="D15">
-        <v>47175169</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B19" s="3">
+        <v>20</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E19" s="3">
+        <v>47175428</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C16">
-        <v>0.03</v>
-      </c>
-      <c r="D16">
-        <v>47175169</v>
-      </c>
-      <c r="E16">
-        <v>-17102.3</v>
-      </c>
-      <c r="F16">
-        <v>182.774</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C17">
-        <v>0.03</v>
-      </c>
-      <c r="D17">
-        <v>47175169</v>
-      </c>
-      <c r="E17">
-        <v>-17058.259999999998</v>
-      </c>
-      <c r="F17">
-        <v>149.58099999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B20" s="3">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E20" s="3">
+        <v>47175428</v>
+      </c>
+      <c r="F20" s="3">
+        <v>-17682.32</v>
+      </c>
+      <c r="G20" s="3">
+        <v>113.0896</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E21" s="3">
+        <v>47175428</v>
+      </c>
+      <c r="F21" s="3">
+        <v>-17663.14</v>
+      </c>
+      <c r="G21" s="3">
+        <v>137.374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18">
-        <v>0.09</v>
-      </c>
-      <c r="C18">
-        <v>0.03</v>
-      </c>
-      <c r="D18">
-        <v>47175426</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B22" s="1">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E22" s="1">
+        <v>47475424</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19">
-        <v>0.09</v>
-      </c>
-      <c r="C19">
-        <v>0.03</v>
-      </c>
-      <c r="D19">
-        <v>47175428</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B23" s="1">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E23" s="1">
+        <v>47475425</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>0.09</v>
-      </c>
-      <c r="C20">
-        <v>0.03</v>
-      </c>
-      <c r="D20">
-        <v>47175428</v>
-      </c>
-      <c r="E20">
-        <v>-17682.32</v>
-      </c>
-      <c r="F20">
-        <v>113.0896</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>0.09</v>
-      </c>
-      <c r="C21">
-        <v>0.03</v>
-      </c>
-      <c r="D21">
-        <v>47175428</v>
-      </c>
-      <c r="E21">
-        <v>-17663.14</v>
-      </c>
-      <c r="F21">
-        <v>137.374</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E24" s="1">
+        <v>47475425</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E25" s="1">
+        <v>47475425</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -931,15 +1148,15 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -953,7 +1170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -970,7 +1187,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -987,7 +1204,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1004,7 +1221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1021,7 +1238,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I6" t="s">
         <v>10</v>
       </c>
@@ -1029,7 +1246,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I7" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
         <v>14</v>
       </c>

</xml_diff>